<commit_message>
implemented UV sensor, took out carrier shift pot (47k res instead), changed UV_OUT pin, some other stuff, added level shifter for ublox gps tcd and rxd lines, added low voltage detection,\n added no gps data reset function to attempt to fix problem
</commit_message>
<xml_diff>
--- a/Current Consumption of Arduino.xlsx
+++ b/Current Consumption of Arduino.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ric\Desktop\UNI\Electronics And Telecommuncations Bach\Year 3\4. Research Project (Thur)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9A0826-7C92-456B-9A81-EA67A4FCD183}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220B2F68-A293-4CBC-9EB8-5B2A7147359A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{20B5EE07-143B-4D59-BC3E-89FEF79D2587}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Component</t>
   </si>
@@ -102,6 +102,30 @@
   </si>
   <si>
     <t>400mA USB or 900mA External if VIN=7V</t>
+  </si>
+  <si>
+    <t>GPS_LOCK_LED</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>[MEASURED] Total current through 3V3 pin = 39mA (OK)</t>
+  </si>
+  <si>
+    <t>[MEASURED] Total current through 5V pin = 17.5mA (OK)</t>
+  </si>
+  <si>
+    <t>[MEASURED] Total current through USB VCC = 110mA (AVERAGE, OK)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Arduino UNO</t>
+  </si>
+  <si>
+    <t>22.6mA (no LEDs expt ON_LED) -&gt; 48mA (L led blink on)</t>
   </si>
 </sst>
 </file>
@@ -199,13 +223,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E92722D-FC4A-4A8E-8AFF-0878AC84B04F}" name="Table1" displayName="Table1" ref="A1:F16" totalsRowShown="0" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E92722D-FC4A-4A8E-8AFF-0878AC84B04F}" name="Table1" displayName="Table1" ref="A1:F16" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:F16" xr:uid="{68374396-69D1-4124-89AC-4B199CD4CCD6}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C5D859CD-BE10-439E-A6FA-2786829FF419}" name="Pin" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{D700EEF1-EF76-4B5F-8520-DE006B30D35C}" name="Pin Max Allowable Consumption" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{AAF1F944-242F-43D5-B822-DB79FA76E54D}" name="Component" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{06A9C260-62BC-4E37-8C24-DF500D4B5851}" name="Voltage (V)" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{C5D859CD-BE10-439E-A6FA-2786829FF419}" name="Pin" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{D700EEF1-EF76-4B5F-8520-DE006B30D35C}" name="Pin Max Allowable Consumption" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{AAF1F944-242F-43D5-B822-DB79FA76E54D}" name="Component" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{06A9C260-62BC-4E37-8C24-DF500D4B5851}" name="Voltage (V)" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{F9A78EF1-9E55-4562-A241-2975CC47D1CB}" name="Current Consumption (mA)" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{C50BF3EE-7AA3-4E72-A35C-FE82FA5E3123}" name="Current Total (mA)" dataDxfId="0">
       <calculatedColumnFormula>SUM(E:E)</calculatedColumnFormula>
@@ -515,7 +539,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,7 +590,7 @@
       </c>
       <c r="F2" s="3">
         <f t="shared" ref="F2:F16" si="0">SUM(E:E)</f>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -587,7 +611,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -608,7 +632,7 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -629,7 +653,7 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -650,18 +674,28 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>15.2</v>
+      </c>
       <c r="F7" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -672,18 +706,28 @@
       <c r="E8" s="1"/>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -694,40 +738,46 @@
       <c r="E10" s="1"/>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -738,7 +788,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -749,7 +799,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -760,7 +810,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="3">
         <f t="shared" si="0"/>
-        <v>108.3</v>
+        <v>123.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>